<commit_message>
making read xlsx better
</commit_message>
<xml_diff>
--- a/data/task01/plant_matrerial_2023.xlsx
+++ b/data/task01/plant_matrerial_2023.xlsx
@@ -193,10 +193,10 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.1"/>
   </cols>
@@ -292,7 +292,7 @@
         <v>202302</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>

</xml_diff>